<commit_message>
Allow technical lifetimes to reduce to 5
</commit_message>
<xml_diff>
--- a/analysis/4_run_message/scenarios.xlsx
+++ b/analysis/4_run_message/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\analysis\4_run_message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BAA5EBA-15EC-449F-A7BA-A89DA0522A7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E481B200-AC23-4FF0-8799-652CAEDA8824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5953306A-3E49-4D6C-A95F-65BD8AD6FB69}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8145" xr2:uid="{5953306A-3E49-4D6C-A95F-65BD8AD6FB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="49">
   <si>
     <t>MESSAGE-TRADE Scenario and Version</t>
   </si>
@@ -66,6 +66,117 @@
   </si>
   <si>
     <t>Switch out oil_exp parameters with oil_exp_'R' parameters</t>
+  </si>
+  <si>
+    <t>Parameterize all oil_exp</t>
+  </si>
+  <si>
+    <t>Start time</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>Add all regions oil_exp_'r' technology, keep oil_exp</t>
+  </si>
+  <si>
+    <t>Add only oil_exp_cpa technology, keep oil_exp</t>
+  </si>
+  <si>
+    <t>Add all regions oil_exp_'r' technology, remove oil_exp</t>
+  </si>
+  <si>
+    <t>MESSAGEix_SSP3</t>
+  </si>
+  <si>
+    <t>Back to: Add all regions oil_exp_'r' technology, keep oil_exp</t>
+  </si>
+  <si>
+    <t>Back to: Add all regions oil_exp_'r' technology, keep oil_exp *I actually kept oil_exp out by mistake</t>
+  </si>
+  <si>
+    <t>Back to: Add only oil_exp_cpa technology, keep oil_exp (re-doing since I upgraded message)</t>
+  </si>
+  <si>
+    <t>Back to: Add all regions oil_exp_'r' technology, keep oil_exp (I updated CPLEX to run Barrier method)</t>
+  </si>
+  <si>
+    <t>Back to: Add all regions oil_exp_'r' technology, remove oil_exp (I updated CPLEX to run Barrier method)</t>
+  </si>
+  <si>
+    <t>MESSAGEix_SSP4</t>
+  </si>
+  <si>
+    <t>Add all regions oil_exp_'r' technology, remove oil_exp, change boundary conditions so that upper and lower are very different</t>
+  </si>
+  <si>
+    <t>Fix activity bounds so that historic values are included</t>
+  </si>
+  <si>
+    <t>Fix activity bounds so that shares are BY YEAR, not just BY COUNTRY!</t>
+  </si>
+  <si>
+    <t>Fix growth boundaries, historical activity, historical new capacity</t>
+  </si>
+  <si>
+    <t>Add import parameters, otherwise commodity balance not met</t>
+  </si>
+  <si>
+    <t>Add import parameters, otherwise commodity balance not met, add back original oil_exp</t>
+  </si>
+  <si>
+    <t>Add import parameters, otherwise commodity balance not met, add back original oil_imp</t>
+  </si>
+  <si>
+    <t>Remove oil_imp and oil_exp, include all new technologies (oil)</t>
+  </si>
+  <si>
+    <t>Remove oil_imp and oil_exp, include all new technologies (oil)+fix historical export input parameter</t>
+  </si>
+  <si>
+    <t>Make 40 year constraint on output and input 20 years</t>
+  </si>
+  <si>
+    <t>MESSAGEix_SSP5</t>
+  </si>
+  <si>
+    <t>Make input parameter for oil_exp technologies 1.1</t>
+  </si>
+  <si>
+    <t>Technical lifetime of oil technologies to 25</t>
+  </si>
+  <si>
+    <t>Add relation_activity for oil_exp_'r' technologies</t>
+  </si>
+  <si>
+    <t>Add technical lifetime for when region of technology (oil_exp_'region') is the node_loc</t>
+  </si>
+  <si>
+    <t>Add relation_activity, ref_new_capacity, ref_activity for oil_exp and oil_imp technologies</t>
+  </si>
+  <si>
+    <t>Make activity bounds larger</t>
+  </si>
+  <si>
+    <t>Remove EEU, keep oil_exp and oil_imp</t>
+  </si>
+  <si>
+    <t>Make activity bounds much larger (add 10e8), remove oil_exp and oil_imp technologies</t>
+  </si>
+  <si>
+    <t>Remove activity bounds</t>
+  </si>
+  <si>
+    <t>Remove activity bounds, technical lifetime to 10</t>
+  </si>
+  <si>
+    <t>Remove activity bounds, allow inputs to go to 10 years (include 10 years)</t>
+  </si>
+  <si>
+    <t>Change commodity name (crudeoil_region to crudeoil)</t>
+  </si>
+  <si>
+    <t>Change commodity name, make export technologies no vintage</t>
   </si>
 </sst>
 </file>
@@ -117,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -162,20 +273,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8478204-7BB5-4095-9E62-D455880F0DDA}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,35 +628,41 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="97.28515625" customWidth="1"/>
+    <col min="6" max="6" width="115.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -550,6 +680,661 @@
       </c>
       <c r="F3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.71319444444444446</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.47291666666666665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>